<commit_message>
- Schema changes - #121 Custom validatio for Russian identity documents type
</commit_message>
<xml_diff>
--- a/DatabaseUpdate/ExcelFiles/InsuranceDocumentTypes.xlsx
+++ b/DatabaseUpdate/ExcelFiles/InsuranceDocumentTypes.xlsx
@@ -1,90 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ChildCare\DatabaseUpdate\ExcelFiles\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
-  </bookViews>
-  <sheets>
-    <sheet name="InsuranceDocumentTypes Data" sheetId="2" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="0"/>
-</workbook>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:workbookPr codeName="ThisWorkbook"/>
+  <x:bookViews>
+    <x:workbookView firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Data" sheetId="2" r:id="rId2"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="125725"/>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Полис</t>
-  </si>
-  <si>
-    <t>Бумажка</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <x:si>
+    <x:t>Id</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Полис</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Бумажка</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="1">
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+</x:styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -367,41 +377,46 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-</worksheet>
+<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B3"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:2">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:2">
+      <x:c r="A2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:2">
+      <x:c r="A3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>